<commit_message>
Finalização da tabela de trabalhos relacionados
Alteração de texto e finalização da tabela de trabalhos relacionados
</commit_message>
<xml_diff>
--- a/Documentação/Tabela_Trabalhos_Relacionados.xlsx
+++ b/Documentação/Tabela_Trabalhos_Relacionados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MeusProjetos\Trabalho-de-Graduacao\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9966675E-D89E-43E1-9E41-26396FE0047D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12014929-5D3F-4AC4-A54C-C7EBC6A3DCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{AD57AB2D-0E31-4FC9-8EDF-4EE0427B97FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD57AB2D-0E31-4FC9-8EDF-4EE0427B97FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Pontos Positivos</t>
   </si>
@@ -119,13 +119,19 @@
   <si>
     <t>Aplicaram a inteligência artificial na àrea da saúde;
 Realizaram a leitura de pontos de referência também para o corpo;</t>
+  </si>
+  <si>
+    <t>Autores não relataram pontos de dificuldade ou melhorias.</t>
+  </si>
+  <si>
+    <t>Trabalho não se enquadra como pesquisa científica.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +154,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -406,6 +420,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -415,22 +444,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,68 +763,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D435936C-75EC-4B54-8F8E-BD88A1F1291E}">
   <dimension ref="B1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="57" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="8" width="11.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -822,7 +833,9 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
@@ -833,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -856,7 +869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -875,9 +888,11 @@
       <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -892,9 +907,11 @@
       <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -921,7 +938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
@@ -938,7 +955,9 @@
       <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Adição de Estrutura de Dados
Adicionado tópico de Estrutura de Dados, além de referências, correções de formatações ABNT e atualização de quadros.
</commit_message>
<xml_diff>
--- a/Documentação/Tabela_Trabalhos_Relacionados.xlsx
+++ b/Documentação/Tabela_Trabalhos_Relacionados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MeusProjetos\Trabalho-de-Graduacao\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12014929-5D3F-4AC4-A54C-C7EBC6A3DCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A23AF-218D-4277-BA24-28D1614635D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD57AB2D-0E31-4FC9-8EDF-4EE0427B97FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Pontos Positivos</t>
   </si>
@@ -64,30 +64,6 @@
   </si>
   <si>
     <t>Implementou efetivamente técnicas para criar uma base de dados bem estruturada;</t>
-  </si>
-  <si>
-    <t>Tópicos correlatos</t>
-  </si>
-  <si>
-    <t>Libras</t>
-  </si>
-  <si>
-    <t>MediaPipe</t>
-  </si>
-  <si>
-    <t>TensorFlow</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>OpenCV</t>
-  </si>
-  <si>
-    <t>Criação de Base de Dados</t>
-  </si>
-  <si>
-    <t>Python</t>
   </si>
   <si>
     <t>Desenvolveram uma documentação robusta de utilização da ferramenta;</t>
@@ -125,13 +101,46 @@
   </si>
   <si>
     <t>Trabalho não se enquadra como pesquisa científica.</t>
+  </si>
+  <si>
+    <t>Tópicos Correlatos</t>
+  </si>
+  <si>
+    <t>Criação de Base de Dados;
+Libras;
+Tensorflow; 
+Python;</t>
+  </si>
+  <si>
+    <t>Criação de Base de Dados; 
+Libras; 
+Python;</t>
+  </si>
+  <si>
+    <t>MediaPipe; 
+Tensorflow; 
+Python;</t>
+  </si>
+  <si>
+    <t>OpenCV;</t>
+  </si>
+  <si>
+    <t>Libras; 
+OpenCV; 
+MediaPipe; 
+Tensorflow; 
+Python;</t>
+  </si>
+  <si>
+    <t>Criação de Base de Dados; 
+Python;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,21 +151,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -177,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -220,76 +214,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -377,6 +301,101 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -388,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -396,55 +415,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -761,211 +774,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D435936C-75EC-4B54-8F8E-BD88A1F1291E}">
-  <dimension ref="B1:J9"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="8" width="11.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>1</v>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="19" t="s">
+    <row r="7" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="19" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="8" spans="2:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="2" t="s">
+      <c r="E8" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="C2:H2"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao tópico Estrutura de Dados
Continuação do tópico de Estrutura de Dados, atualização de referências, figuras e outras correções
</commit_message>
<xml_diff>
--- a/Documentação/Tabela_Trabalhos_Relacionados.xlsx
+++ b/Documentação/Tabela_Trabalhos_Relacionados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MeusProjetos\Trabalho-de-Graduacao\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A23AF-218D-4277-BA24-28D1614635D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4699D815-6F8A-475D-8095-56AD9C3C19A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD57AB2D-0E31-4FC9-8EDF-4EE0427B97FD}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Cruz (2020)</t>
   </si>
   <si>
-    <t>Nascimento e Teles ()</t>
-  </si>
-  <si>
     <t>Marengoni e Stringhini (2009)</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   <si>
     <t>Criação de Base de Dados; 
 Python;</t>
+  </si>
+  <si>
+    <t>Nascimento et al. (2020)</t>
   </si>
 </sst>
 </file>
@@ -777,13 +777,13 @@
   <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42" style="1" bestFit="1" customWidth="1"/>
@@ -793,10 +793,10 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>0</v>
@@ -810,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -824,69 +824,69 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>